<commit_message>
updates to variable names and cleaning code
</commit_message>
<xml_diff>
--- a/ca-brfss_varnames.xlsx
+++ b/ca-brfss_varnames.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lamhine/Documents/GitHub/brfss_disagg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E004C7C2-1FC6-DC48-9E1C-63CF6F9A0539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDB2334-225D-8C41-9F45-F6708D00D632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{A3B2E6ED-C6DE-B048-8453-B086D8E72AFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="230">
   <si>
     <t>alcohol consumption</t>
   </si>
@@ -510,13 +511,229 @@
   </si>
   <si>
     <t>EVER DIAGNOSED WITH HEART ATTACK</t>
+  </si>
+  <si>
+    <t>_RFBMI5</t>
+  </si>
+  <si>
+    <t>OVERWEIGHT OR OBESE CALCULATED VARIABLE</t>
+  </si>
+  <si>
+    <t>lung cancer screening</t>
+  </si>
+  <si>
+    <t>EXERANY2</t>
+  </si>
+  <si>
+    <t>EXERCISE IN PAST 30 DAYS</t>
+  </si>
+  <si>
+    <t>EXERANY1</t>
+  </si>
+  <si>
+    <t>ANY PHYSICAL ACTIVITY OTHER THAN JOB</t>
+  </si>
+  <si>
+    <t>COMPUTED SMOKING STATUS</t>
+  </si>
+  <si>
+    <t>_SMOKER3</t>
+  </si>
+  <si>
+    <t>USE OF SMOKELESS TOBACCO PRODUCTS</t>
+  </si>
+  <si>
+    <t>USENOW3</t>
+  </si>
+  <si>
+    <t>CURRENTLY USE CHEWING TOBACCO, SNUFF, OR SNUS</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>education</t>
+  </si>
+  <si>
+    <t>employment</t>
+  </si>
+  <si>
+    <t>income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hearing </t>
+  </si>
+  <si>
+    <t>internet</t>
+  </si>
+  <si>
+    <t>marital status</t>
+  </si>
+  <si>
+    <t>number of children</t>
+  </si>
+  <si>
+    <t>race</t>
+  </si>
+  <si>
+    <t>rent/own home</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>veteran status</t>
+  </si>
+  <si>
+    <t>AGE</t>
+  </si>
+  <si>
+    <t>1984-2020</t>
+  </si>
+  <si>
+    <t>REPORTED AGE IN YEARS</t>
+  </si>
+  <si>
+    <t>difficulty concentrating</t>
+  </si>
+  <si>
+    <t>DECIDE</t>
+  </si>
+  <si>
+    <t>REMEM2</t>
+  </si>
+  <si>
+    <t>DIFFICULTY CONCENTRATING, REMEMBERING, MAKING DECISIONS</t>
+  </si>
+  <si>
+    <t>DIFFICULTY CONCENTRATING OR REMEMBERING</t>
+  </si>
+  <si>
+    <t>difficulty with errands</t>
+  </si>
+  <si>
+    <t>DIFFERND</t>
+  </si>
+  <si>
+    <t>DIFFICULTY DOING ERRANDS BECAUSE OF PHYSICAL, MENTAL, EMOTIONAL CONDITION</t>
+  </si>
+  <si>
+    <t>DIFFICULTY DOING ERRANDS ALONE</t>
+  </si>
+  <si>
+    <t>DIFFALON</t>
+  </si>
+  <si>
+    <t>difficulty dressing or bathing</t>
+  </si>
+  <si>
+    <t>DIFDRES2</t>
+  </si>
+  <si>
+    <t>DIFFICULTY DRESSING OR BATHING</t>
+  </si>
+  <si>
+    <t>DIFFDRES</t>
+  </si>
+  <si>
+    <t>difficulty walking/stairs</t>
+  </si>
+  <si>
+    <t>DIFFWALK</t>
+  </si>
+  <si>
+    <t>DIFFICULTY WALKING OR CLIMBING STAIRS</t>
+  </si>
+  <si>
+    <t>EDUCAC</t>
+  </si>
+  <si>
+    <t>EDUCATION LEVEL (CDC CATEGORIES)</t>
+  </si>
+  <si>
+    <t>EDUCA</t>
+  </si>
+  <si>
+    <t>EDUCATION LEVEL</t>
+  </si>
+  <si>
+    <t>EMPLOY1</t>
+  </si>
+  <si>
+    <t>EMPLOYMENT STATUS</t>
+  </si>
+  <si>
+    <t>EMPLOY2</t>
+  </si>
+  <si>
+    <t>HOUSEHOLD INCOME-CDC CODE</t>
+  </si>
+  <si>
+    <t>INCOME3</t>
+  </si>
+  <si>
+    <t>INCOME LEVEL</t>
+  </si>
+  <si>
+    <t>MARITAL</t>
+  </si>
+  <si>
+    <t>MARITAL STATUS</t>
+  </si>
+  <si>
+    <t>_CHLDCNT</t>
+  </si>
+  <si>
+    <t>NUMBER OF CHILDREN IN HOUSEHOLD</t>
+  </si>
+  <si>
+    <t>COMPUTED NUMBER OF CHILDREN IN HOUSEHOLD</t>
+  </si>
+  <si>
+    <t>RENTHOM1</t>
+  </si>
+  <si>
+    <t>OWN OR RENT HOME</t>
+  </si>
+  <si>
+    <t>COLGSEX1</t>
+  </si>
+  <si>
+    <t>ARE YOU MALE OR FEMALE?</t>
+  </si>
+  <si>
+    <t>SEX, SEX1, SEX2</t>
+  </si>
+  <si>
+    <t>SEX ASSIGNED TO YOU AT BIRTH, ON BIRTH CERTIFICATE</t>
+  </si>
+  <si>
+    <t>_IMPHOME</t>
+  </si>
+  <si>
+    <t>IMPUTED RENT OR OWN HOME STATUS</t>
+  </si>
+  <si>
+    <t>INCOM02</t>
+  </si>
+  <si>
+    <t>OWNHOME</t>
+  </si>
+  <si>
+    <t>BIRTHSEX</t>
+  </si>
+  <si>
+    <t>FLUSHOT6,FLUSHOT7</t>
+  </si>
+  <si>
+    <t>INCOM02, INCOM03</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -531,13 +748,25 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -552,12 +781,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -892,25 +1124,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22E5723B-F729-BC48-9949-E1832937859F}">
-  <dimension ref="A1:L58"/>
+  <dimension ref="A1:L75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="75.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="61.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E1" s="1">
+      <c r="E1" s="5">
         <v>2022</v>
       </c>
-      <c r="F1" s="1"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
@@ -988,7 +1218,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E5" t="s">
@@ -1017,7 +1247,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D6" t="s">
@@ -1049,7 +1279,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F7" t="s">
@@ -1075,12 +1305,12 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E9" t="s">
@@ -1359,22 +1589,22 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="1" t="s">
         <v>101</v>
       </c>
       <c r="H18" t="s">
@@ -1470,7 +1700,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E21" t="s">
@@ -1499,32 +1729,32 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1709,7 +1939,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1718,7 +1948,7 @@
         <v>31</v>
       </c>
       <c r="B38" t="s">
-        <v>143</v>
+        <v>228</v>
       </c>
       <c r="C38" t="s">
         <v>84</v>
@@ -1754,98 +1984,423 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="A41" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="A42" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="A43" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="A44" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" t="s">
+        <v>158</v>
+      </c>
+      <c r="C48" t="s">
+        <v>59</v>
+      </c>
+      <c r="D48" t="s">
+        <v>159</v>
+      </c>
+      <c r="E48" t="s">
+        <v>158</v>
+      </c>
+      <c r="F48" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="B50" t="s">
+        <v>163</v>
+      </c>
+      <c r="C50" t="s">
+        <v>67</v>
+      </c>
+      <c r="D50" t="s">
+        <v>164</v>
+      </c>
+      <c r="E50" t="s">
+        <v>161</v>
+      </c>
+      <c r="F50" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+      <c r="B55" t="s">
+        <v>166</v>
+      </c>
+      <c r="C55" t="s">
+        <v>59</v>
+      </c>
+      <c r="D55" t="s">
+        <v>165</v>
+      </c>
+      <c r="E55" t="s">
+        <v>166</v>
+      </c>
+      <c r="F55" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="B56" t="s">
+        <v>168</v>
+      </c>
+      <c r="C56" t="s">
+        <v>81</v>
+      </c>
+      <c r="D56" t="s">
+        <v>169</v>
+      </c>
+      <c r="E56" t="s">
+        <v>168</v>
+      </c>
+      <c r="F56" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B60" t="s">
+        <v>182</v>
+      </c>
+      <c r="C60" t="s">
+        <v>183</v>
+      </c>
+      <c r="D60" t="s">
+        <v>184</v>
+      </c>
+      <c r="E60" t="s">
+        <v>182</v>
+      </c>
+      <c r="F60" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B61" t="s">
+        <v>187</v>
+      </c>
+      <c r="C61" t="s">
+        <v>91</v>
+      </c>
+      <c r="D61" t="s">
+        <v>188</v>
+      </c>
+      <c r="E61" t="s">
+        <v>186</v>
+      </c>
+      <c r="F61" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B62" t="s">
+        <v>191</v>
+      </c>
+      <c r="C62" t="s">
+        <v>91</v>
+      </c>
+      <c r="D62" t="s">
+        <v>192</v>
+      </c>
+      <c r="E62" t="s">
+        <v>194</v>
+      </c>
+      <c r="F62" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B63" t="s">
+        <v>196</v>
+      </c>
+      <c r="C63" t="s">
+        <v>91</v>
+      </c>
+      <c r="D63" t="s">
+        <v>197</v>
+      </c>
+      <c r="E63" t="s">
+        <v>198</v>
+      </c>
+      <c r="F63" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B64" t="s">
+        <v>200</v>
+      </c>
+      <c r="C64" t="s">
+        <v>91</v>
+      </c>
+      <c r="D64" t="s">
+        <v>201</v>
+      </c>
+      <c r="E64" t="s">
+        <v>200</v>
+      </c>
+      <c r="F64" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B65" t="s">
+        <v>202</v>
+      </c>
+      <c r="C65" t="s">
+        <v>59</v>
+      </c>
+      <c r="D65" t="s">
+        <v>203</v>
+      </c>
+      <c r="E65" t="s">
+        <v>204</v>
+      </c>
+      <c r="F65" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B66" t="s">
+        <v>208</v>
+      </c>
+      <c r="C66" t="s">
+        <v>127</v>
+      </c>
+      <c r="D66" t="s">
+        <v>207</v>
+      </c>
+      <c r="E66" t="s">
+        <v>206</v>
+      </c>
+      <c r="F66" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B70" t="s">
+        <v>212</v>
+      </c>
+      <c r="C70" t="s">
+        <v>183</v>
+      </c>
+      <c r="D70" t="s">
+        <v>213</v>
+      </c>
+      <c r="E70" t="s">
+        <v>212</v>
+      </c>
+      <c r="F70" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B71" t="s">
+        <v>214</v>
+      </c>
+      <c r="C71" t="s">
+        <v>59</v>
+      </c>
+      <c r="D71" t="s">
+        <v>215</v>
+      </c>
+      <c r="E71" t="s">
+        <v>214</v>
+      </c>
+      <c r="F71" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B73" t="s">
+        <v>226</v>
+      </c>
+      <c r="C73" t="s">
+        <v>59</v>
+      </c>
+      <c r="D73" t="s">
+        <v>224</v>
+      </c>
+      <c r="E73" t="s">
+        <v>217</v>
+      </c>
+      <c r="F73" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B74" t="s">
+        <v>221</v>
+      </c>
+      <c r="C74" t="s">
+        <v>183</v>
+      </c>
+      <c r="D74" t="s">
+        <v>222</v>
+      </c>
+      <c r="E74" t="s">
+        <v>227</v>
+      </c>
+      <c r="F74" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -1854,4 +2409,511 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0C6A679-1ABB-1244-8FAF-0481D831C9F3}">
+  <dimension ref="A1:D72"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="str">
+        <f>A1&amp;", "&amp;B1</f>
+        <v>DRNKANY5, DRNKANY6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="str">
+        <f>A2&amp;", "&amp;B2</f>
+        <v>_RFBING5, _RFBING6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" ref="D8:D18" si="0">A8&amp;", "&amp;B8</f>
+        <v>ASTHEVE3, ASTHMA3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>ASTHNOW, ASTHNOW</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>ANGINA, CVDCRHD4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>153</v>
+      </c>
+      <c r="B11" t="s">
+        <v>156</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>HEART2, CVDINFR4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>COPDEVER, CHCCOPD3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>DEPRESS1, ADDEPEV3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>DIABCOR3, DIABETE4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>KIDNEY, CHCKDNY2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>SKCANC, CHCSCNC1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>BLIND, BLIND</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" t="s">
+        <v>111</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" ref="D26:D34" si="1">A26&amp;", "&amp;B26</f>
+        <v>HAVEPLN3, _HLTHPLN</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>113</v>
+      </c>
+      <c r="B27" t="s">
+        <v>115</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="1"/>
+        <v>CHECKUP2, CHECKUP1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28" t="s">
+        <v>117</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="1"/>
+        <v>PERSDOC, PERSDOC3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>122</v>
+      </c>
+      <c r="B29" t="s">
+        <v>124</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="1"/>
+        <v>_HCVU651, _HCVU652</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" t="s">
+        <v>126</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="1"/>
+        <v>GENHLTH, GENHLTH</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" t="s">
+        <v>126</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="1"/>
+        <v>GENHLTH, GENHLTH</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>131</v>
+      </c>
+      <c r="B32" t="s">
+        <v>131</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="1"/>
+        <v>PHYSHLTH, PHYSHLTH</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>135</v>
+      </c>
+      <c r="B33" t="s">
+        <v>135</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="1"/>
+        <v>MENTHLTH, MENTHLTH</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>140</v>
+      </c>
+      <c r="B34" t="s">
+        <v>138</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="1"/>
+        <v>AIDSTST8,AIDSTST9, HIVTST7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>143</v>
+      </c>
+      <c r="B36" t="s">
+        <v>146</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" ref="D36:D37" si="2">A36&amp;", "&amp;B36</f>
+        <v>FLUSHOT5,FLUSHOT6,FLUSHOT7, FLUSHOT7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>147</v>
+      </c>
+      <c r="B37" t="s">
+        <v>151</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="2"/>
+        <v>PNEUMVC3,PNEUMVC4, PNEUVAC4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>158</v>
+      </c>
+      <c r="B46" t="s">
+        <v>158</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" ref="D46" si="3">A46&amp;", "&amp;B46</f>
+        <v>_RFBMI5, _RFBMI5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>163</v>
+      </c>
+      <c r="B48" t="s">
+        <v>161</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" ref="D48" si="4">A48&amp;", "&amp;B48</f>
+        <v>EXERANY1, EXERANY2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>166</v>
+      </c>
+      <c r="B53" t="s">
+        <v>166</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" ref="D53:D54" si="5">A53&amp;", "&amp;B53</f>
+        <v>_SMOKER3, _SMOKER3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>168</v>
+      </c>
+      <c r="B54" t="s">
+        <v>168</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="5"/>
+        <v>USENOW3, USENOW3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>182</v>
+      </c>
+      <c r="B58" t="s">
+        <v>182</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" ref="D58:D65" si="6">A58&amp;", "&amp;B58</f>
+        <v>AGE, AGE</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>187</v>
+      </c>
+      <c r="B59" t="s">
+        <v>186</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="6"/>
+        <v>REMEM2, DECIDE</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>191</v>
+      </c>
+      <c r="B60" t="s">
+        <v>194</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="6"/>
+        <v>DIFFERND, DIFFALON</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>196</v>
+      </c>
+      <c r="B61" t="s">
+        <v>198</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="6"/>
+        <v>DIFDRES2, DIFFDRES</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>200</v>
+      </c>
+      <c r="B62" t="s">
+        <v>200</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="6"/>
+        <v>DIFFWALK, DIFFWALK</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>202</v>
+      </c>
+      <c r="B63" t="s">
+        <v>204</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="6"/>
+        <v>EDUCAC, EDUCA</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>208</v>
+      </c>
+      <c r="B64" t="s">
+        <v>206</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="6"/>
+        <v>EMPLOY2, EMPLOY1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="6"/>
+        <v>INCOM02, INCOME3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>212</v>
+      </c>
+      <c r="B68" t="s">
+        <v>212</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" ref="D68:D69" si="7">A68&amp;", "&amp;B68</f>
+        <v>MARITAL, MARITAL</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>214</v>
+      </c>
+      <c r="B69" t="s">
+        <v>214</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" si="7"/>
+        <v>_CHLDCNT, _CHLDCNT</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>223</v>
+      </c>
+      <c r="B71" t="s">
+        <v>217</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" ref="D71:D72" si="8">A71&amp;", "&amp;B71</f>
+        <v>_IMPHOME, RENTHOM1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>221</v>
+      </c>
+      <c r="B72" t="s">
+        <v>219</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" si="8"/>
+        <v>SEX, SEX1, SEX2, COLGSEX1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>